<commit_message>
NEW FEATURE: BW CarbRatios decoded
</commit_message>
<xml_diff>
--- a/doc/Events_log_decoded.xlsx
+++ b/doc/Events_log_decoded.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all_events" sheetId="1" r:id="rId1"/>
     <sheet name="Arrow status mapping" sheetId="2" r:id="rId2"/>
+    <sheet name="Carb ratios" sheetId="3" r:id="rId3"/>
+    <sheet name="Sensitivity factors" sheetId="5" r:id="rId4"/>
+    <sheet name="BG Targets" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="423">
   <si>
     <t>_id</t>
   </si>
@@ -1223,13 +1226,81 @@
   </si>
   <si>
     <t>46 rate of change (2)</t>
+  </si>
+  <si>
+    <t>03012C2E7007000000000000019000000000000000044C0B000000000000044C11000000000000044C13000000000000028A1600000000000001F41E00000000000001F424</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>PREAMBLE</t>
+  </si>
+  <si>
+    <t>COMMAND</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>REC1</t>
+  </si>
+  <si>
+    <t>REC2</t>
+  </si>
+  <si>
+    <t>REC3</t>
+  </si>
+  <si>
+    <t>REC4</t>
+  </si>
+  <si>
+    <t>REC5</t>
+  </si>
+  <si>
+    <t>REC6</t>
+  </si>
+  <si>
+    <t>REC7</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04012F1AB7050096005300007800430C00640038140078004324008C004E2E
+</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">050132D1E10400780043005A003200007800430050002C0A007800430050002C1000780043005A003224
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1373,6 +1444,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -1730,7 +1806,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1755,6 +1831,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1802,6 +1888,25 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="60">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2269,7 +2374,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2504,42 +2608,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2877,6 +2945,24 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2891,81 +2977,81 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BF109" totalsRowShown="0" headerRowDxfId="40" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:BF109" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:BF109"/>
   <tableColumns count="58">
-    <tableColumn id="1" name="_id" dataDxfId="59"/>
-    <tableColumn id="2" name="timestamp" dataDxfId="58"/>
-    <tableColumn id="3" name="type" dataDxfId="57"/>
-    <tableColumn id="4" name="statusRaw" dataDxfId="56"/>
-    <tableColumn id="5" name="hour" dataDxfId="54"/>
-    <tableColumn id="39" name="03 - pump status (1)" dataDxfId="22">
+    <tableColumn id="1" name="_id" dataDxfId="57"/>
+    <tableColumn id="2" name="timestamp" dataDxfId="56"/>
+    <tableColumn id="3" name="type" dataDxfId="55"/>
+    <tableColumn id="4" name="statusRaw" dataDxfId="54"/>
+    <tableColumn id="5" name="hour" dataDxfId="53"/>
+    <tableColumn id="39" name="03 - pump status (1)" dataDxfId="52">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(F$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(F$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" name="???" dataDxfId="15">
+    <tableColumn id="46" name="???" dataDxfId="51">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],1,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" name="cgm" dataDxfId="14">
+    <tableColumn id="45" name="cgm" dataDxfId="50">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],2,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" name="temp basal" dataDxfId="21">
+    <tableColumn id="44" name="temp basal" dataDxfId="49">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],3,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" name="ins. del." dataDxfId="20">
+    <tableColumn id="43" name="ins. del." dataDxfId="48">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],4,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" name="bol. dual" dataDxfId="19">
+    <tableColumn id="42" name="bol. dual" dataDxfId="47">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],5,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="bol. square" dataDxfId="18">
+    <tableColumn id="41" name="bol. square" dataDxfId="46">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],6,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="47" name="bol. Normal" dataDxfId="17">
+    <tableColumn id="47" name="bol. Normal" dataDxfId="45">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],7,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="suspended" dataDxfId="16">
+    <tableColumn id="40" name="suspended" dataDxfId="44">
       <calculatedColumnFormula>MID(Table1[[#This Row],[03 - pump status (1)]],8,1)="1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" name="04 - now bolusing (4)" dataDxfId="13">
+    <tableColumn id="48" name="04 - now bolusing (4)" dataDxfId="43">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(O$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" name="08 - ?? (4)" dataDxfId="12">
+    <tableColumn id="49" name="08 - ?? (4)" dataDxfId="42">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(P$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" name="0C - NM (2)" dataDxfId="11">
+    <tableColumn id="51" name="0C - NM (2)" dataDxfId="41">
       <calculatedColumnFormula>" 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Q$1,2))*2, 4) &amp; " " &amp; IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Q$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Q$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Q$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" name="0E - NR (2)" dataDxfId="10">
+    <tableColumn id="50" name="0E - NR (2)" dataDxfId="40">
       <calculatedColumnFormula>" 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(R$1,2))*2, 4) &amp; " " &amp; IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(R$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(R$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(R$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" name="10 - last bolus amount (4)" dataDxfId="9">
+    <tableColumn id="52" name="10 - last bolus amount (4)" dataDxfId="39">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(S$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" name="14 - last bolus time (4)" dataDxfId="1">
+    <tableColumn id="53" name="14 - last bolus time (4)" dataDxfId="38">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(T$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="54" name="18 - last bolus ref. (2)" dataDxfId="8">
+    <tableColumn id="54" name="18 - last bolus ref. (2)" dataDxfId="37">
       <calculatedColumnFormula>" 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(U$1,2))*2, 4) &amp; " " &amp; IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(U$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(U$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(U$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="55" name="1A - basal pattern (1)" dataDxfId="7">
+    <tableColumn id="55" name="1A - basal pattern (1)" dataDxfId="36">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(V$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(V$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="56" name="1B - basal rate (4)" dataDxfId="6">
+    <tableColumn id="56" name="1B - basal rate (4)" dataDxfId="35">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(W$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="57" name="1F -temp basal rate (4)" dataDxfId="5">
+    <tableColumn id="57" name="1F -temp basal rate (4)" dataDxfId="34">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(X$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" name="24 - temp. min (2)" dataDxfId="4">
+    <tableColumn id="58" name="24 - temp. min (2)" dataDxfId="33">
       <calculatedColumnFormula>IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Y$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Y$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Y$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="26 - basal units/day  (4)" dataDxfId="23">
+    <tableColumn id="38" name="26 - basal units/day  (4)" dataDxfId="32">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(Z$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="2A - battery (1)" dataDxfId="24">
+    <tableColumn id="37" name="2A - battery (1)" dataDxfId="31">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AA$1,2))*2, 2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" name="2B - res. insulin (4)2" dataDxfId="27">
+    <tableColumn id="36" name="2B - res. insulin (4)2" dataDxfId="30">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AB$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" name="2F - res. hours (1)" dataDxfId="29">
@@ -2974,88 +3060,88 @@
     <tableColumn id="34" name="30 - res. min (1)" dataDxfId="28">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AD$1,2))*2, 2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="31 - active insulin (4)" dataDxfId="33">
+    <tableColumn id="33" name="31 - active insulin (4)" dataDxfId="27">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AE$1,2))*2, 8))/10000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="35 - SGV (2)" dataDxfId="2">
+    <tableColumn id="14" name="35 - SGV (2)" dataDxfId="26">
       <calculatedColumnFormula>IF(AND(Table1[[#This Row],[cgm]],NOT(Table1[[#This Row],[35 - SGV special bit (2)]])), _xlfn.BITAND(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AF$1,2))*2, 4)),HEX2DEC("1FF")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="59" name="35 - SGV special bit (2)" dataDxfId="3">
+    <tableColumn id="59" name="35 - SGV special bit (2)" dataDxfId="25">
       <calculatedColumnFormula>_xlfn.BITAND(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AG$1,2))*2, 4)),512)=512</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="37 - sgv time (4)2" dataDxfId="53">
+    <tableColumn id="15" name="37 - sgv time (4)2" dataDxfId="24">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AF$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="3B - sgv time offst (4)" dataDxfId="52">
+    <tableColumn id="16" name="3B - sgv time offst (4)" dataDxfId="23">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AH$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="3F - low susp (1)" dataDxfId="51">
+    <tableColumn id="17" name="3F - low susp (1)" dataDxfId="22">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AJ$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AJ$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="40 trend" dataDxfId="50">
+    <tableColumn id="7" name="40 trend" dataDxfId="21">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AK$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AK$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="trend" dataDxfId="49">
+    <tableColumn id="9" name="trend" dataDxfId="20">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[40 trend]],'Arrow status mapping'!$A$1:$B$8,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="41 status (1)" dataDxfId="48">
+    <tableColumn id="18" name="41 status (1)" dataDxfId="19">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AM$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AM$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="42 control (1)" dataDxfId="47">
+    <tableColumn id="19" name="42 control (1)" dataDxfId="18">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AN$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AN$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="43 calib time remaining" dataDxfId="46">
+    <tableColumn id="13" name="43 calib time remaining" dataDxfId="17">
       <calculatedColumnFormula>" 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AO$1,2))*2, 4) &amp; " " &amp; IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AO$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AO$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AO$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="45 battery" dataDxfId="45">
+    <tableColumn id="6" name="45 battery" dataDxfId="16">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AP$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AP$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="46 rate of change (2)" dataDxfId="44">
+    <tableColumn id="8" name="46 rate of change (2)" dataDxfId="15">
       <calculatedColumnFormula>" 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AQ$1,2))*2, 4) &amp; " " &amp; IF(HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AQ$1,2))*2, 4))&gt;32768,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AQ$1,2))*2, 4))-65536,HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AQ$1,2))*2, 4)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="calc rate of change" dataDxfId="43">
+    <tableColumn id="10" name="calc rate of change" dataDxfId="14">
       <calculatedColumnFormula>TRUNC(_xlfn.NUMBERVALUE(RIGHT(Table1[[#This Row],[46 rate of change (2)]],LEN(Table1[[#This Row],[46 rate of change (2)]])-7))/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="calc arrow" dataDxfId="42">
+    <tableColumn id="11" name="calc arrow" dataDxfId="13">
       <calculatedColumnFormula>IF(Table1[[#This Row],[calc rate of change]]&gt;0,Table1[[#This Row],[calc rate of change]]&amp;" arrows up",IF(Table1[[#This Row],[calc rate of change]]&lt;0,(0-Table1[[#This Row],[calc rate of change]])&amp;" arrows down","No arrows"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="comp" dataDxfId="41">
+    <tableColumn id="12" name="comp" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[calc arrow]]=Table1[[#This Row],[trend]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="48 bolus wizard ?" dataDxfId="39">
+    <tableColumn id="20" name="48 bolus wizard ?" dataDxfId="11">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AU$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AU$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="49 - BGV (2)" dataDxfId="0">
+    <tableColumn id="21" name="49 - BGV (2)" dataDxfId="10">
       <calculatedColumnFormula>HEX2DEC(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AV$1,2))*2, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="4B Alerts1 (1)" dataDxfId="38">
+    <tableColumn id="23" name="4B Alerts1 (1)" dataDxfId="9">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AW$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AW$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="4C Alerts2 (1)" dataDxfId="37">
+    <tableColumn id="24" name="4C Alerts2 (1)" dataDxfId="8">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AX$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AX$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="4D - alert time (4)" dataDxfId="31">
+    <tableColumn id="25" name="4D - alert time (4)" dataDxfId="7">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AY$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="51 - alert time offst (4)" dataDxfId="30">
+    <tableColumn id="26" name="51 - alert time offst (4)" dataDxfId="6">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(AZ$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="55 ???" dataDxfId="36">
+    <tableColumn id="27" name="55 ???" dataDxfId="5">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BA$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BA$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="56 ???" dataDxfId="35">
+    <tableColumn id="28" name="56 ???" dataDxfId="4">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BB$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BB$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="57 ???" dataDxfId="34">
+    <tableColumn id="29" name="57 ???" dataDxfId="3">
       <calculatedColumnFormula>HEX2BIN(MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BC$1,2))*2, 2),8) &amp; " 0x" &amp;MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BC$1,2))*2, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="58 - sensor active (4)2" dataDxfId="32">
+    <tableColumn id="30" name="58 - sensor active (4)2" dataDxfId="2">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BD$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" name="5C - sensor active (4)" dataDxfId="26">
+    <tableColumn id="31" name="5C - sensor active (4)" dataDxfId="1">
       <calculatedColumnFormula>MID(Table1[[#This Row],[statusRaw]],1+HEX2DEC(LEFT(BE$1,2))*2, 8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="Comments / observations" dataDxfId="25"/>
+    <tableColumn id="32" name="Comments / observations" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3326,7 +3412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AI1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
@@ -28071,4 +28157,1156 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B4)*2,2*HEX2DEC(C4))</f>
+        <v>03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+HEX2DEC(C4),2)</f>
+        <v>01</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B5)*2,2*HEX2DEC(C5))</f>
+        <v>012C</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="16" t="str">
+        <f t="shared" ref="B6:B14" si="0">DEC2HEX(HEX2DEC(B5)+HEX2DEC(C5),2)</f>
+        <v>03</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B6)*2,2*HEX2DEC(C6))</f>
+        <v>2E70</v>
+      </c>
+      <c r="E6">
+        <f>HEX2DEC(D6)</f>
+        <v>11888</v>
+      </c>
+      <c r="F6">
+        <f>HEX2DEC(MID(D6,1,2))</f>
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <f>HEX2DEC(MID(D6,3,2))</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>05</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B7)*2,2*HEX2DEC(C7))</f>
+        <v>07</v>
+      </c>
+      <c r="E7">
+        <f>HEX2DEC(D7)</f>
+        <v>7</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>409</v>
+      </c>
+      <c r="B8" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>06</v>
+      </c>
+      <c r="C8" s="16">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" ref="D8:D14" si="1">MID($A$1,1+HEX2DEC(B8)*2,2*HEX2DEC(C8))</f>
+        <v>000000000000019000</v>
+      </c>
+      <c r="E8" t="str">
+        <f>MID(D8,13,4)</f>
+        <v>0190</v>
+      </c>
+      <c r="F8">
+        <f>HEX2DEC(E8)/1000</f>
+        <v>0.4</v>
+      </c>
+      <c r="G8" t="str">
+        <f>RIGHT(D8,2)</f>
+        <v>00</v>
+      </c>
+      <c r="H8">
+        <f>HEX2DEC(G8)/2</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="L8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>0F</v>
+      </c>
+      <c r="C9" s="16">
+        <f>C8</f>
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>000000000000044C0B</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9:E14" si="2">MID(D9,13,4)</f>
+        <v>044C</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F14" si="3">HEX2DEC(E9)/1000</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" ref="G9:G14" si="4">RIGHT(D9,2)</f>
+        <v>0B</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H14" si="5">HEX2DEC(G9)/2</f>
+        <v>5.5</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="L9">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="16">
+        <f t="shared" ref="C10:C14" si="6">C9</f>
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>000000000000044C11</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>044C</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>8.5</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="L10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>412</v>
+      </c>
+      <c r="B11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>000000000000044C13</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>044C</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>9.5</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="L11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>413</v>
+      </c>
+      <c r="B12" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>2A</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>000000000000028A16</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>028A</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K12" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="L12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>414</v>
+      </c>
+      <c r="B13" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C13" s="16">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000001F41E</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>01F4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="4"/>
+        <v>1E</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="K13" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="L13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>415</v>
+      </c>
+      <c r="B14" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>3C</v>
+      </c>
+      <c r="C14" s="16">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>00000000000001F424</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>01F4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B4)*2,2*HEX2DEC(C4))</f>
+        <v>04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+HEX2DEC(C4),2)</f>
+        <v>01</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B5)*2,2*HEX2DEC(C5))</f>
+        <v>012F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="16" t="str">
+        <f t="shared" ref="B6:B13" si="0">DEC2HEX(HEX2DEC(B5)+HEX2DEC(C5),2)</f>
+        <v>03</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B6)*2,2*HEX2DEC(C6))</f>
+        <v>1AB7</v>
+      </c>
+      <c r="E6">
+        <f>HEX2DEC(D6)</f>
+        <v>6839</v>
+      </c>
+      <c r="F6">
+        <f>HEX2DEC(MID(D6,1,2))</f>
+        <v>26</v>
+      </c>
+      <c r="G6">
+        <f>HEX2DEC(MID(D6,3,2))</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>05</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B7)*2,2*HEX2DEC(C7))</f>
+        <v>05</v>
+      </c>
+      <c r="E7">
+        <f>HEX2DEC(D7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>409</v>
+      </c>
+      <c r="B9" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(B7)+HEX2DEC(C7),2)</f>
+        <v>06</v>
+      </c>
+      <c r="C9" s="16">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" ref="D9:D13" si="1">MID($A$1,1+HEX2DEC(B9)*2,2*HEX2DEC(C9))</f>
+        <v>0096005300</v>
+      </c>
+      <c r="E9" t="str">
+        <f>MID(D9,1,4)</f>
+        <v>0096</v>
+      </c>
+      <c r="F9">
+        <f>HEX2DEC(E9)</f>
+        <v>150</v>
+      </c>
+      <c r="G9" t="str">
+        <f>RIGHT(D9,2)</f>
+        <v>00</v>
+      </c>
+      <c r="H9">
+        <f>HEX2DEC(G9)/2</f>
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <f>MID(D9,5,4)</f>
+        <v>0053</v>
+      </c>
+      <c r="J9">
+        <f>HEX2DEC(I9)</f>
+        <v>83</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>0B</v>
+      </c>
+      <c r="C10" s="16">
+        <f>C9</f>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>007800430C</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" ref="E10:E13" si="2">MID(D10,1,4)</f>
+        <v>0078</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:F13" si="3">HEX2DEC(E10)</f>
+        <v>120</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10:G13" si="4">RIGHT(D10,2)</f>
+        <v>0C</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H13" si="5">HEX2DEC(G10)/2</f>
+        <v>6</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ref="I10:I13" si="6">MID(D10,5,4)</f>
+        <v>0043</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J13" si="7">HEX2DEC(I10)</f>
+        <v>67</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="M10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" ref="C11:C13" si="8">C10</f>
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0064003814</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>0064</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="6"/>
+        <v>0038</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="7"/>
+        <v>56</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B12" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0078004324</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>0078</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="6"/>
+        <v>0043</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="7"/>
+        <v>67</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="M12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>413</v>
+      </c>
+      <c r="B13" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="C13" s="16">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>008C004E2E</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>008C</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="4"/>
+        <v>2E</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="6"/>
+        <v>004E</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="M13">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="165" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B4)*2,2*HEX2DEC(C4))</f>
+        <v>05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(B4)+HEX2DEC(C4),2)</f>
+        <v>01</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B5)*2,2*HEX2DEC(C5))</f>
+        <v>0132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" s="16" t="str">
+        <f t="shared" ref="B6:B7" si="0">DEC2HEX(HEX2DEC(B5)+HEX2DEC(C5),2)</f>
+        <v>03</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B6)*2,2*HEX2DEC(C6))</f>
+        <v>D1E1</v>
+      </c>
+      <c r="E6">
+        <f>HEX2DEC(D6)</f>
+        <v>53729</v>
+      </c>
+      <c r="F6">
+        <f>HEX2DEC(MID(D6,1,2))</f>
+        <v>209</v>
+      </c>
+      <c r="G6">
+        <f>HEX2DEC(MID(D6,3,2))</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>05</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(B7)*2,2*HEX2DEC(C7))</f>
+        <v>04</v>
+      </c>
+      <c r="E7">
+        <f>HEX2DEC(D7)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="K8" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>120</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="E9" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(B7)+HEX2DEC(C7),2)</f>
+        <v>06</v>
+      </c>
+      <c r="F9" s="16">
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(E9)*2,2*HEX2DEC(F9))</f>
+        <v>00780043005A003200</v>
+      </c>
+      <c r="H9" t="str">
+        <f>RIGHT(G9,2)</f>
+        <v>00</v>
+      </c>
+      <c r="I9">
+        <f>HEX2DEC(H9)/2</f>
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f>MID(G9,1,4)</f>
+        <v>0078</v>
+      </c>
+      <c r="K9">
+        <f>HEX2DEC(J9)</f>
+        <v>120</v>
+      </c>
+      <c r="L9" t="str">
+        <f>MID(G9,5,4)</f>
+        <v>0043</v>
+      </c>
+      <c r="M9">
+        <f>HEX2DEC(L9)</f>
+        <v>67</v>
+      </c>
+      <c r="N9" t="str">
+        <f>MID(G9,9,4)</f>
+        <v>005A</v>
+      </c>
+      <c r="O9">
+        <f>HEX2DEC(N9)</f>
+        <v>90</v>
+      </c>
+      <c r="P9" t="str">
+        <f>MID(G9,13,4)</f>
+        <v>0032</v>
+      </c>
+      <c r="Q9">
+        <f>HEX2DEC(P9)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>120</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="E10" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(E9)+HEX2DEC(F9),2)</f>
+        <v>0F</v>
+      </c>
+      <c r="F10" s="16">
+        <f>F9</f>
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(E10)*2,2*HEX2DEC(F10))</f>
+        <v>007800430050002C0A</v>
+      </c>
+      <c r="H10" t="str">
+        <f>RIGHT(G10,2)</f>
+        <v>0A</v>
+      </c>
+      <c r="I10">
+        <f>HEX2DEC(H10)/2</f>
+        <v>5</v>
+      </c>
+      <c r="J10" t="str">
+        <f>MID(G10,1,4)</f>
+        <v>0078</v>
+      </c>
+      <c r="K10">
+        <f>HEX2DEC(J10)</f>
+        <v>120</v>
+      </c>
+      <c r="L10" t="str">
+        <f>MID(G10,5,4)</f>
+        <v>0043</v>
+      </c>
+      <c r="M10">
+        <f>HEX2DEC(L10)</f>
+        <v>67</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" ref="N10:N12" si="1">MID(G10,9,4)</f>
+        <v>0050</v>
+      </c>
+      <c r="O10">
+        <f>HEX2DEC(N10)</f>
+        <v>80</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" ref="P10:P12" si="2">MID(G10,13,4)</f>
+        <v>002C</v>
+      </c>
+      <c r="Q10">
+        <f>HEX2DEC(P10)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="E11" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(E10)+HEX2DEC(F10),2)</f>
+        <v>18</v>
+      </c>
+      <c r="F11" s="16">
+        <f>F10</f>
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(E11)*2,2*HEX2DEC(F11))</f>
+        <v>007800430050002C10</v>
+      </c>
+      <c r="H11" t="str">
+        <f>RIGHT(G11,2)</f>
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f>HEX2DEC(H11)/2</f>
+        <v>8</v>
+      </c>
+      <c r="J11" t="str">
+        <f>MID(G11,1,4)</f>
+        <v>0078</v>
+      </c>
+      <c r="K11">
+        <f>HEX2DEC(J11)</f>
+        <v>120</v>
+      </c>
+      <c r="L11" t="str">
+        <f>MID(G11,5,4)</f>
+        <v>0043</v>
+      </c>
+      <c r="M11">
+        <f>HEX2DEC(L11)</f>
+        <v>67</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>0050</v>
+      </c>
+      <c r="O11">
+        <f>HEX2DEC(N11)</f>
+        <v>80</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="2"/>
+        <v>002C</v>
+      </c>
+      <c r="Q11">
+        <f>HEX2DEC(P11)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="E12" s="16" t="str">
+        <f>DEC2HEX(HEX2DEC(E11)+HEX2DEC(F11),2)</f>
+        <v>21</v>
+      </c>
+      <c r="F12" s="16">
+        <f>F11</f>
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="str">
+        <f>MID($A$1,1+HEX2DEC(E12)*2,2*HEX2DEC(F12))</f>
+        <v>00780043005A003224</v>
+      </c>
+      <c r="H12" t="str">
+        <f>RIGHT(G12,2)</f>
+        <v>24</v>
+      </c>
+      <c r="I12">
+        <f>HEX2DEC(H12)/2</f>
+        <v>18</v>
+      </c>
+      <c r="J12" t="str">
+        <f>MID(G12,1,4)</f>
+        <v>0078</v>
+      </c>
+      <c r="K12">
+        <f>HEX2DEC(J12)</f>
+        <v>120</v>
+      </c>
+      <c r="L12" t="str">
+        <f>MID(G12,5,4)</f>
+        <v>0043</v>
+      </c>
+      <c r="M12">
+        <f>HEX2DEC(L12)</f>
+        <v>67</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>005A</v>
+      </c>
+      <c r="O12">
+        <f>HEX2DEC(N12)</f>
+        <v>90</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>0032</v>
+      </c>
+      <c r="Q12">
+        <f>HEX2DEC(P12)</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>